<commit_message>
task 7 og 10
</commit_message>
<xml_diff>
--- a/Data/winequality-red.xlsx
+++ b/Data/winequality-red.xlsx
@@ -82,7 +82,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -655,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
         <v>7.4</v>
       </c>
@@ -693,7 +693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="9">
         <v>7.8</v>
       </c>
@@ -731,7 +731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="9">
         <v>7.8</v>
       </c>
@@ -769,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="9">
         <v>11.2</v>
       </c>
@@ -807,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="9">
         <v>7.4</v>
       </c>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="9">
         <v>7.4</v>
       </c>
@@ -883,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="9">
         <v>7.9</v>
       </c>
@@ -921,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="9">
         <v>7.3</v>
       </c>
@@ -959,7 +959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="9">
         <v>7.8</v>
       </c>
@@ -997,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="9">
         <v>7.5</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="9">
         <v>6.7</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="9">
         <v>7.5</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="9">
         <v>5.6</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="9">
         <v>7.8</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="9">
         <v>8.9</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="9">
         <v>8.9</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="9">
         <v>8.5</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="9">
         <v>8.1</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="9">
         <v>7.4</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="9">
         <v>7.9</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="9">
         <v>8.9</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="9">
         <v>7.6</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.05">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="9">
         <v>7.9</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.05">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="9">
         <v>8.5</v>
       </c>

</xml_diff>